<commit_message>
added excess_energy_price to batching
</commit_message>
<xml_diff>
--- a/data/simulation_input.xlsx
+++ b/data/simulation_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineriksson/PycharmProjects/Simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCB70D9-2FC5-CC41-91FA-BA21A814F8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB88773-F5E6-544F-B485-4A79C4530575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4820" yWindow="24000" windowWidth="28040" windowHeight="17440" xr2:uid="{8D530716-A5A5-884E-A1EF-2775436591A8}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
removed hydro pump and changed it to 12h bess in xlsx
</commit_message>
<xml_diff>
--- a/data/simulation_input.xlsx
+++ b/data/simulation_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineriksson/PycharmProjects/Simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45B45B8-71EC-A640-8F95-AFF8936E20E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513C462D-7EF7-484F-9BAA-5F118518B167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4820" yWindow="24000" windowWidth="28040" windowHeight="17440" xr2:uid="{8D530716-A5A5-884E-A1EF-2775436591A8}"/>
   </bookViews>
@@ -86,10 +86,10 @@
     <t>battery_8h_price</t>
   </si>
   <si>
-    <t>hydro_storage_price</t>
-  </si>
-  <si>
-    <t>hydro_storage_mw</t>
+    <t>battery_12h_mw</t>
+  </si>
+  <si>
+    <t>battery_12h_price</t>
   </si>
 </sst>
 </file>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7B980E-8246-6D4A-AA5E-C7CBF5A2A6AD}">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,10 +550,10 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
         <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>